<commit_message>
feat [04/05]: update CiteSeer model
</commit_message>
<xml_diff>
--- a/hardware/data/citeseer/data.xlsx
+++ b/hardware/data/citeseer/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\New Model\CiteSeer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Capstone\Project\Graph-Attention-Network-FPGA\software\benchmark\Model\CiteSeer\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F50768-4BBF-490B-9CA1-D60A729868D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698968C1-369F-4DD3-81AC-4DEF9135B20C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{55869166-5A30-41E5-9330-ED053189522E}"/>
   </bookViews>
@@ -150,7 +150,7 @@
     <t>COEF remove còn 2 bits</t>
   </si>
   <si>
-    <t>New feature remove còn 7 bits</t>
+    <t>New feature remove còn 8 bits</t>
   </si>
 </sst>
 </file>
@@ -344,21 +344,72 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -366,57 +417,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -756,7 +756,7 @@
   <dimension ref="C6:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -771,30 +771,30 @@
   </cols>
   <sheetData>
     <row r="6" spans="3:14">
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="24" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="28"/>
-      <c r="K6" s="29"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="22"/>
       <c r="L6" s="9"/>
-      <c r="M6" s="30" t="s">
+      <c r="M6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="31"/>
+      <c r="N6" s="24"/>
     </row>
     <row r="7" spans="3:14">
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="32"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="5" t="s">
         <v>3</v>
       </c>
@@ -817,10 +817,10 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="3:14">
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="32"/>
+      <c r="D8" s="25"/>
       <c r="E8" s="5" t="s">
         <v>4</v>
       </c>
@@ -843,56 +843,56 @@
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="3:14">
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="25" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="32">
         <v>13264</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="39"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="34"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="36">
+      <c r="I9" s="29">
         <v>12383</v>
       </c>
-      <c r="J9" s="37"/>
-      <c r="K9" s="38"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="31"/>
       <c r="L9" s="12"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="3:14">
-      <c r="C10" s="32"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="32">
         <v>169</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="39"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="34"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="36">
+      <c r="I10" s="29">
         <v>100</v>
       </c>
-      <c r="J10" s="37"/>
-      <c r="K10" s="38"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="31"/>
       <c r="L10" s="12"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
     <row r="11" spans="3:14">
-      <c r="C11" s="32"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="32">
         <v>242101</v>
       </c>
-      <c r="F11" s="20"/>
+      <c r="F11" s="33"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="10">
@@ -905,7 +905,7 @@
       <c r="N11" s="3"/>
     </row>
     <row r="12" spans="3:14">
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="25" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -914,52 +914,52 @@
       <c r="E12" s="5">
         <v>508</v>
       </c>
-      <c r="F12" s="21"/>
+      <c r="F12" s="38"/>
       <c r="G12" s="5">
         <v>79682</v>
       </c>
-      <c r="H12" s="21"/>
+      <c r="H12" s="38"/>
       <c r="I12" s="10">
-        <v>739</v>
-      </c>
-      <c r="J12" s="16">
+        <v>733</v>
+      </c>
+      <c r="J12" s="35">
         <v>10</v>
       </c>
       <c r="K12" s="10">
-        <v>32062</v>
-      </c>
-      <c r="L12" s="16">
+        <v>32994</v>
+      </c>
+      <c r="L12" s="35">
         <v>16</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="3:14">
-      <c r="C13" s="32"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="5">
         <v>-485</v>
       </c>
-      <c r="F13" s="23"/>
+      <c r="F13" s="40"/>
       <c r="G13" s="5">
         <v>-43443</v>
       </c>
-      <c r="H13" s="23"/>
+      <c r="H13" s="40"/>
       <c r="I13" s="10">
-        <v>-450</v>
-      </c>
-      <c r="J13" s="18"/>
+        <v>-673</v>
+      </c>
+      <c r="J13" s="36"/>
       <c r="K13" s="10">
-        <v>-9985</v>
-      </c>
-      <c r="L13" s="18"/>
+        <v>-16086</v>
+      </c>
+      <c r="L13" s="36"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
     <row r="14" spans="3:14">
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="26" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -968,152 +968,152 @@
       <c r="E14" s="5">
         <v>141129</v>
       </c>
-      <c r="F14" s="21"/>
+      <c r="F14" s="38"/>
       <c r="G14" s="5">
         <v>7771420</v>
       </c>
-      <c r="H14" s="21"/>
+      <c r="H14" s="38"/>
       <c r="I14" s="10">
-        <v>25940</v>
-      </c>
-      <c r="J14" s="16">
+        <v>374177</v>
+      </c>
+      <c r="J14" s="35">
         <v>20</v>
       </c>
       <c r="K14" s="10">
-        <v>4071874</v>
-      </c>
-      <c r="L14" s="16">
+        <v>4132334</v>
+      </c>
+      <c r="L14" s="35">
         <v>23</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
     <row r="15" spans="3:14">
-      <c r="C15" s="34"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="5">
         <v>-122985</v>
       </c>
-      <c r="F15" s="22"/>
+      <c r="F15" s="39"/>
       <c r="G15" s="5">
         <v>-15780793</v>
       </c>
-      <c r="H15" s="22"/>
+      <c r="H15" s="39"/>
       <c r="I15" s="10">
-        <v>-20535</v>
-      </c>
-      <c r="J15" s="17"/>
+        <v>-74526</v>
+      </c>
+      <c r="J15" s="37"/>
       <c r="K15" s="10">
-        <v>-322221</v>
-      </c>
-      <c r="L15" s="17"/>
+        <v>-2593188</v>
+      </c>
+      <c r="L15" s="37"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
     <row r="16" spans="3:14">
-      <c r="C16" s="34"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="5">
         <v>188808</v>
       </c>
-      <c r="F16" s="22"/>
+      <c r="F16" s="39"/>
       <c r="G16" s="5">
         <v>11502871</v>
       </c>
-      <c r="H16" s="22"/>
+      <c r="H16" s="39"/>
       <c r="I16" s="10">
-        <v>32522</v>
-      </c>
-      <c r="J16" s="17"/>
+        <v>426247</v>
+      </c>
+      <c r="J16" s="37"/>
       <c r="K16" s="10">
-        <v>4284833</v>
-      </c>
-      <c r="L16" s="17"/>
+        <v>4428335</v>
+      </c>
+      <c r="L16" s="37"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
     <row r="17" spans="3:14">
-      <c r="C17" s="34"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
       </c>
-      <c r="F17" s="23"/>
+      <c r="F17" s="40"/>
       <c r="G17" s="5">
         <v>0</v>
       </c>
-      <c r="H17" s="23"/>
+      <c r="H17" s="40"/>
       <c r="I17" s="10">
         <v>0</v>
       </c>
-      <c r="J17" s="18"/>
+      <c r="J17" s="36"/>
       <c r="K17" s="10">
         <v>0</v>
       </c>
-      <c r="L17" s="18"/>
+      <c r="L17" s="36"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
     <row r="18" spans="3:14">
-      <c r="C18" s="34"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E18" s="5">
         <v>2</v>
       </c>
-      <c r="F18" s="21"/>
+      <c r="F18" s="38"/>
       <c r="G18" s="5">
         <v>2</v>
       </c>
-      <c r="H18" s="21"/>
+      <c r="H18" s="38"/>
       <c r="I18" s="10">
         <v>1</v>
       </c>
-      <c r="J18" s="16">
+      <c r="J18" s="35">
         <v>8</v>
       </c>
       <c r="K18" s="10">
         <v>1</v>
       </c>
-      <c r="L18" s="16">
+      <c r="L18" s="35">
         <v>8</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="3:14">
-      <c r="C19" s="34"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E19" s="5">
         <v>0</v>
       </c>
-      <c r="F19" s="23"/>
+      <c r="F19" s="40"/>
       <c r="G19" s="5">
         <v>0</v>
       </c>
-      <c r="H19" s="23"/>
+      <c r="H19" s="40"/>
       <c r="I19" s="10">
         <v>0</v>
       </c>
-      <c r="J19" s="18"/>
+      <c r="J19" s="36"/>
       <c r="K19" s="10">
         <v>0</v>
       </c>
-      <c r="L19" s="18"/>
+      <c r="L19" s="36"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
     <row r="20" spans="3:14">
-      <c r="C20" s="35"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="2" t="s">
         <v>34</v>
       </c>
@@ -1135,7 +1135,7 @@
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="3:14">
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="26" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -1149,11 +1149,11 @@
         <v>4</v>
       </c>
       <c r="H21" s="8"/>
-      <c r="I21" s="40">
+      <c r="I21" s="16">
         <v>2</v>
       </c>
       <c r="J21" s="13"/>
-      <c r="K21" s="40">
+      <c r="K21" s="16">
         <v>2</v>
       </c>
       <c r="L21" s="13"/>
@@ -1161,7 +1161,7 @@
       <c r="N21" s="3"/>
     </row>
     <row r="22" spans="3:14">
-      <c r="C22" s="34"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1185,7 +1185,7 @@
       <c r="N22" s="3"/>
     </row>
     <row r="23" spans="3:14">
-      <c r="C23" s="34"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="2" t="s">
         <v>21</v>
       </c>
@@ -1197,11 +1197,11 @@
         <v>329</v>
       </c>
       <c r="H23" s="8"/>
-      <c r="I23" s="40">
+      <c r="I23" s="16">
         <v>100</v>
       </c>
       <c r="J23" s="13"/>
-      <c r="K23" s="40">
+      <c r="K23" s="16">
         <v>100</v>
       </c>
       <c r="L23" s="13"/>
@@ -1209,7 +1209,7 @@
       <c r="N23" s="3"/>
     </row>
     <row r="24" spans="3:14">
-      <c r="C24" s="34"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1233,7 +1233,7 @@
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="3:14">
-      <c r="C25" s="34"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="2" t="s">
         <v>23</v>
       </c>
@@ -1246,7 +1246,7 @@
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="10">
-        <v>0.66666666666666596</v>
+        <v>0.5</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10">
@@ -1257,7 +1257,7 @@
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="3:14">
-      <c r="C26" s="35"/>
+      <c r="C26" s="28"/>
       <c r="D26" s="2" t="s">
         <v>24</v>
       </c>
@@ -1269,11 +1269,11 @@
         <v>3.0395136778115501E-3</v>
       </c>
       <c r="H26" s="8"/>
-      <c r="I26" s="40">
+      <c r="I26" s="16">
         <v>0.01</v>
       </c>
       <c r="J26" s="13"/>
-      <c r="K26" s="40">
+      <c r="K26" s="16">
         <v>0.01</v>
       </c>
       <c r="L26" s="13"/>
@@ -1281,7 +1281,7 @@
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="3:14">
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="25" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -1296,18 +1296,18 @@
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="10">
-        <v>465.75</v>
+        <v>629.66666666666595</v>
       </c>
       <c r="J27" s="10"/>
       <c r="K27" s="10">
-        <v>27374.5</v>
+        <v>28308.571428571398</v>
       </c>
       <c r="L27" s="10"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
     </row>
     <row r="28" spans="3:14">
-      <c r="C28" s="32"/>
+      <c r="C28" s="25"/>
       <c r="D28" s="2" t="s">
         <v>7</v>
       </c>
@@ -1342,6 +1342,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="L14:L17"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="J14:J17"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H16:H17"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="M6:N6"/>
@@ -1358,19 +1371,6 @@
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="L12:L13"/>
-    <mergeCell ref="L14:L17"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="J14:J17"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="H16:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>